<commit_message>
listo para maestro detalle
</commit_message>
<xml_diff>
--- a/Reportes/ReporteClientes.xlsx
+++ b/Reportes/ReporteClientes.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Rc823e1df160242bf"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Re89c0ccd11b648d0"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -71,7 +71,7 @@
     <x:t>Cherey</x:t>
   </x:si>
   <x:si>
-    <x:t>27889988</x:t>
+    <x:t>27889989</x:t>
   </x:si>
   <x:si>
     <x:t>elen@gmail.com</x:t>
@@ -92,7 +92,7 @@
     <x:t>Roque</x:t>
   </x:si>
   <x:si>
-    <x:t>Rios</x:t>
+    <x:t>Muñoz</x:t>
   </x:si>
   <x:si>
     <x:t>37899878</x:t>

</xml_diff>